<commit_message>
* Adding images for maven and system path variables.
</commit_message>
<xml_diff>
--- a/src/test/resources/testParameters.xlsx
+++ b/src/test/resources/testParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11745"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <t>https://www.yandex.com/</t>
   </si>
   <si>
-    <t>chrome</t>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -39,8 +39,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -61,18 +61,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -91,26 +91,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -130,16 +115,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,6 +145,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -161,16 +169,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,28 +200,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,13 +220,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,163 +346,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,6 +419,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -480,15 +489,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -508,15 +508,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -529,125 +529,125 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -977,7 +977,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>